<commit_message>
Update new sheet log from #28
</commit_message>
<xml_diff>
--- a/new_sheet.xlsx
+++ b/new_sheet.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,6 +475,38 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>edit1</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Merged</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>desc</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2025-06-17</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update new sheet log from #31
</commit_message>
<xml_diff>
--- a/new_sheet.xlsx
+++ b/new_sheet.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -485,6 +485,38 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>edit2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Merged</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>comment!</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2025-06-18</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update new sheet log from #32
</commit_message>
<xml_diff>
--- a/new_sheet.xlsx
+++ b/new_sheet.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -517,6 +517,33 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>edit2</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Merged</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2025-06-18</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update new sheet log from #33
</commit_message>
<xml_diff>
--- a/new_sheet.xlsx
+++ b/new_sheet.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -544,6 +544,33 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>edit2</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Merged</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2025-06-18</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update new sheet log from #34
</commit_message>
<xml_diff>
--- a/new_sheet.xlsx
+++ b/new_sheet.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -571,6 +571,33 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>edit1</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Merged</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2025-06-18</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update new sheet log from #35
</commit_message>
<xml_diff>
--- a/new_sheet.xlsx
+++ b/new_sheet.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -598,6 +598,33 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>edit1</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Merged</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2025-06-18</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update new sheet log from #36
</commit_message>
<xml_diff>
--- a/new_sheet.xlsx
+++ b/new_sheet.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -625,6 +625,33 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>edit1</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Merged</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2025-06-18</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update new sheet log from #37
</commit_message>
<xml_diff>
--- a/new_sheet.xlsx
+++ b/new_sheet.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -652,6 +652,33 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>edit1</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Merged</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>2025-06-18</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update new sheet log from #38
</commit_message>
<xml_diff>
--- a/new_sheet.xlsx
+++ b/new_sheet.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -679,6 +679,38 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>edit1</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Squashed</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2 changes</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2025-06-18</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update new sheet log from #39
</commit_message>
<xml_diff>
--- a/new_sheet.xlsx
+++ b/new_sheet.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -711,6 +711,33 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>edit1</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Squashed</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2025-06-18</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update new sheet log from #40
</commit_message>
<xml_diff>
--- a/new_sheet.xlsx
+++ b/new_sheet.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -738,6 +738,33 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>edit1</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Squashed</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2025-06-18</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>8c6ea62a94902a18d223569759b6f9f29a3c340f</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update new sheet log from #42
</commit_message>
<xml_diff>
--- a/new_sheet.xlsx
+++ b/new_sheet.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -765,6 +765,38 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>edit1</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Squashed</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>2025-06-18</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>846895ac8c5fcf9bec1e93cf92bcdf081ff57046</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update new sheet log from #43
</commit_message>
<xml_diff>
--- a/new_sheet.xlsx
+++ b/new_sheet.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -797,6 +797,38 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>edit1</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Squashed</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>2025-06-18</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2efdb7acf2306cf36253f988e5a0ebd5022b326d</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update new sheet log from #44
</commit_message>
<xml_diff>
--- a/new_sheet.xlsx
+++ b/new_sheet.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -829,6 +829,38 @@
         </is>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>edit1</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Merged</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>2025-06-18</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>0298eb9d9af211aa8d48a882c377fe378d42a3d1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update new sheet log from #45
</commit_message>
<xml_diff>
--- a/new_sheet.xlsx
+++ b/new_sheet.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -861,6 +861,38 @@
         </is>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>edit1</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Merged</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>2025-06-18</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>15431bee5d95560e049c0d32a92e0cea477e3ba5</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update new sheet log from #46
</commit_message>
<xml_diff>
--- a/new_sheet.xlsx
+++ b/new_sheet.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -893,6 +893,38 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>edit1</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Merged</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>2025-06-19</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>37dcd755ab7f59fccebf0f22a88d047d73a1c753</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update new sheet log from #47
</commit_message>
<xml_diff>
--- a/new_sheet.xlsx
+++ b/new_sheet.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -925,6 +925,38 @@
         </is>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>edit2</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Merged</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>2025-06-19</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>7d293280560b9ddde7e5a9a9704e8051967a7a1e</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update new sheet log from #48
</commit_message>
<xml_diff>
--- a/new_sheet.xlsx
+++ b/new_sheet.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -957,6 +957,38 @@
         </is>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>edit1</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Merged</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>2025-06-19</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>8b59deccfda5d1e814ac4d6141e02dc3d5f12b19</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update new sheet log from #49
</commit_message>
<xml_diff>
--- a/new_sheet.xlsx
+++ b/new_sheet.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -989,6 +989,38 @@
         </is>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>edit2</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Merged</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>2025-06-19</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>c886f687e6bc4f27615b5182d10b73894e43a993</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update new sheet log from #50
</commit_message>
<xml_diff>
--- a/new_sheet.xlsx
+++ b/new_sheet.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -989,6 +989,38 @@
         </is>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>edit1</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Merged</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>2025-06-19</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>6bd9de3f8a1122122b8fdaf8a1dea58b3a601eed</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update new sheet log from #52
</commit_message>
<xml_diff>
--- a/new_sheet.xlsx
+++ b/new_sheet.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1021,6 +1021,38 @@
         </is>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>edit1</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Merged</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>2025-06-20</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>86572a2432f91c46fb61abbbadbd0d704a70a3e3</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update new sheet log from #53
</commit_message>
<xml_diff>
--- a/new_sheet.xlsx
+++ b/new_sheet.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1053,6 +1053,38 @@
         </is>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>edit1</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Merged</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>2025-06-20</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>2afd94510241569eb7fd682e244e8e2f0d248e42</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update new sheet log from #54
</commit_message>
<xml_diff>
--- a/new_sheet.xlsx
+++ b/new_sheet.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1085,6 +1085,38 @@
         </is>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>edit1</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Merged</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>2025-06-20</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>825d03f72949eefcc7953a7e836efe245eee87bb</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update new sheet log from #55
</commit_message>
<xml_diff>
--- a/new_sheet.xlsx
+++ b/new_sheet.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1117,6 +1117,38 @@
         </is>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>edit1</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Merged</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>2025-06-23</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>7cb3f674f05f8033cb60e20bc0d35a1e90579a4e</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update new sheet log from #56
</commit_message>
<xml_diff>
--- a/new_sheet.xlsx
+++ b/new_sheet.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1149,6 +1149,38 @@
         </is>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>edit1</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Merged</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>compared ad merged</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>2025-06-23</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>fee73b8b8fd20763dbba2cddf9bcd5df07ff197b</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update new sheet log from #57
</commit_message>
<xml_diff>
--- a/new_sheet.xlsx
+++ b/new_sheet.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1021,6 +1021,38 @@
         </is>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>edit1</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Merged</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>change1</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>2025-06-23</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>1cf76dd27c2ae0ba57e39ad101ab17a10e2d488a</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update new sheet log from #58
</commit_message>
<xml_diff>
--- a/new_sheet.xlsx
+++ b/new_sheet.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1053,6 +1053,38 @@
         </is>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>edit1</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>riya-morankar</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Merged</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>cleared</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>2025-06-30</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>d9e149383f13845f5987656bf79fd690e8faab53</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>